<commit_message>
Improvements in the supplier relation.
</commit_message>
<xml_diff>
--- a/inputs/SIMULATION MASTER ING.xlsx
+++ b/inputs/SIMULATION MASTER ING.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4da58a8d6ef66bb8/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Supply-Chain-RL\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="338" documentId="8_{2CB95B17-427F-4156-8030-1E80245912C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A880857-BEA4-49EC-A071-B0B8642C5DA3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D1A3C9-C3F6-4789-AF5E-58A9CEC3FFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{EEB7F1C1-5855-4098-AB38-0E487DBC6C3A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="2" activeTab="3" xr2:uid="{EEB7F1C1-5855-4098-AB38-0E487DBC6C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="SUSTAINABILITY ACTIONS" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="330">
   <si>
     <t>Business Phase</t>
   </si>
@@ -1727,7 +1727,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1742,12 +1742,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2069,21 +2065,21 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="22.1015625" customWidth="1"/>
+    <col min="2" max="2" width="23.1015625" customWidth="1"/>
     <col min="3" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.3125" customWidth="1"/>
+    <col min="6" max="6" width="16.5234375" customWidth="1"/>
+    <col min="7" max="7" width="19.68359375" customWidth="1"/>
+    <col min="8" max="8" width="19.3125" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.41796875" customWidth="1"/>
+    <col min="11" max="11" width="21.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2118,7 +2114,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="117" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2153,7 +2149,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="112.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2188,7 +2184,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="112.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -2223,7 +2219,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="160.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="160.80000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -2258,7 +2254,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="137.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="137.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -2293,7 +2289,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="127.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="127.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -2341,17 +2337,17 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.3125" customWidth="1"/>
+    <col min="2" max="2" width="17.7890625" customWidth="1"/>
+    <col min="3" max="3" width="23.68359375" customWidth="1"/>
+    <col min="4" max="4" width="20.41796875" customWidth="1"/>
+    <col min="5" max="5" width="17.1015625" customWidth="1"/>
+    <col min="6" max="6" width="24.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>133</v>
       </c>
@@ -2371,7 +2367,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="76.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>141</v>
       </c>
@@ -2391,7 +2387,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>147</v>
       </c>
@@ -2411,7 +2407,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="73.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -2431,7 +2427,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="64.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>154</v>
       </c>
@@ -2458,29 +2454,29 @@
       <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.20703125" customWidth="1"/>
+    <col min="2" max="2" width="19.41796875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.5234375" customWidth="1"/>
+    <col min="5" max="5" width="14.7890625" customWidth="1"/>
+    <col min="6" max="6" width="16.41796875" customWidth="1"/>
+    <col min="7" max="7" width="13.7890625" customWidth="1"/>
+    <col min="8" max="8" width="13.41796875" customWidth="1"/>
+    <col min="9" max="9" width="12.7890625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
-    <col min="12" max="12" width="20.5546875" customWidth="1"/>
-    <col min="13" max="13" width="22.6640625" customWidth="1"/>
-    <col min="18" max="18" width="23.6640625" customWidth="1"/>
-    <col min="19" max="19" width="24.77734375" customWidth="1"/>
-    <col min="20" max="20" width="21.33203125" customWidth="1"/>
-    <col min="21" max="21" width="17.5546875" customWidth="1"/>
-    <col min="22" max="22" width="19.109375" customWidth="1"/>
+    <col min="11" max="11" width="20.3125" customWidth="1"/>
+    <col min="12" max="12" width="20.5234375" customWidth="1"/>
+    <col min="13" max="13" width="22.68359375" customWidth="1"/>
+    <col min="18" max="18" width="23.68359375" customWidth="1"/>
+    <col min="19" max="19" width="24.7890625" customWidth="1"/>
+    <col min="20" max="20" width="21.3125" customWidth="1"/>
+    <col min="21" max="21" width="17.5234375" customWidth="1"/>
+    <col min="22" max="22" width="19.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="55.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -2536,7 +2532,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="115.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>54</v>
       </c>
@@ -2592,7 +2588,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="94.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
@@ -2648,7 +2644,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="96" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>60</v>
       </c>
@@ -2704,7 +2700,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="103.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>63</v>
       </c>
@@ -2760,7 +2756,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="98.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>65</v>
       </c>
@@ -2816,7 +2812,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="104.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>67</v>
       </c>
@@ -2866,7 +2862,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="112.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>69</v>
       </c>
@@ -2914,25 +2910,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D59A61A-A02B-4DC6-87B1-77651CE892A3}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R9" sqref="L1:R9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" customWidth="1"/>
-    <col min="15" max="15" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="14.68359375" customWidth="1"/>
+    <col min="12" max="12" width="11.5234375" customWidth="1"/>
+    <col min="13" max="13" width="17.41796875" customWidth="1"/>
+    <col min="14" max="14" width="14.1015625" customWidth="1"/>
+    <col min="15" max="15" width="12.20703125" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" customWidth="1"/>
+    <col min="17" max="17" width="10.41796875" customWidth="1"/>
     <col min="18" max="18" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="32.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>272</v>
       </c>
@@ -2973,7 +2969,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>278</v>
       </c>
@@ -3018,7 +3014,7 @@
         <v>27.45</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="21.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>279</v>
       </c>
@@ -3059,7 +3055,7 @@
         <v>14.64</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="33.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>280</v>
       </c>
@@ -3100,7 +3096,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>281</v>
       </c>
@@ -3141,7 +3137,7 @@
         <v>10.675000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="L6" s="5" t="s">
         <v>280</v>
       </c>
@@ -3164,7 +3160,7 @@
         <v>15.86</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="D7" t="s">
         <v>292</v>
       </c>
@@ -3190,7 +3186,7 @@
         <v>7.32</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="L8" s="5" t="s">
         <v>281</v>
       </c>
@@ -3213,7 +3209,25 @@
         <v>19.824999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>277</v>
+      </c>
       <c r="L9" s="5" t="s">
         <v>281</v>
       </c>
@@ -3236,9 +3250,107 @@
         <v>13.725</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B10" s="9">
+        <f>B2/4</f>
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" ref="C10:F10" si="0">C2/4</f>
+        <v>16.350000000000001</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>11.25</v>
+      </c>
+      <c r="E10" s="9">
+        <f t="shared" si="0"/>
+        <v>10.125</v>
+      </c>
+      <c r="F10" s="9">
+        <f t="shared" si="0"/>
+        <v>4.5750000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B11" s="9">
+        <f t="shared" ref="B11:F11" si="1">B3/4</f>
+        <v>27.375</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="1"/>
+        <v>13.625</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="1"/>
+        <v>9.375</v>
+      </c>
+      <c r="E11" s="9">
+        <f t="shared" si="1"/>
+        <v>8.4375</v>
+      </c>
+      <c r="F11" s="9">
+        <f t="shared" si="1"/>
+        <v>3.8125</v>
+      </c>
       <c r="N11" t="s">
         <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B12" s="9">
+        <f t="shared" ref="B12:F12" si="2">B4/4</f>
+        <v>21.8</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" si="2"/>
+        <v>10.9</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="E12" s="9">
+        <f t="shared" si="2"/>
+        <v>6.75</v>
+      </c>
+      <c r="F12" s="9">
+        <f t="shared" si="2"/>
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B13" s="9">
+        <f t="shared" ref="B13:F13" si="3">B5/4</f>
+        <v>27.375</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" si="3"/>
+        <v>13.625</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="3"/>
+        <v>9.375</v>
+      </c>
+      <c r="E13" s="9">
+        <f t="shared" si="3"/>
+        <v>8.4375</v>
+      </c>
+      <c r="F13" s="9">
+        <f t="shared" si="3"/>
+        <v>3.5625</v>
       </c>
     </row>
   </sheetData>
@@ -3250,21 +3362,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70AE801-453B-4B0C-A71D-8153467A4225}">
   <dimension ref="A2:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="5" max="5" width="42.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="34.41796875" customWidth="1"/>
+    <col min="2" max="2" width="16.7890625" customWidth="1"/>
+    <col min="5" max="5" width="42.41796875" customWidth="1"/>
+    <col min="6" max="6" width="18.89453125" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" customWidth="1"/>
+    <col min="10" max="10" width="16.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14" t="s">
         <v>306</v>
       </c>
@@ -3281,7 +3393,7 @@
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="13" t="s">
         <v>293</v>
       </c>
@@ -3306,7 +3418,7 @@
       </c>
       <c r="K3" s="14"/>
     </row>
-    <row r="4" spans="1:11" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>295</v>
       </c>
@@ -3331,7 +3443,7 @@
       </c>
       <c r="K4" s="14"/>
     </row>
-    <row r="5" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>297</v>
       </c>
@@ -3356,7 +3468,7 @@
       </c>
       <c r="K5" s="14"/>
     </row>
-    <row r="6" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>298</v>
       </c>
@@ -3381,7 +3493,7 @@
       </c>
       <c r="K6" s="14"/>
     </row>
-    <row r="7" spans="1:11" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="33.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>300</v>
       </c>
@@ -3406,7 +3518,7 @@
       </c>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>301</v>
       </c>
@@ -3431,7 +3543,7 @@
       </c>
       <c r="K8" s="14"/>
     </row>
-    <row r="9" spans="1:11" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>302</v>
       </c>
@@ -3456,7 +3568,7 @@
       </c>
       <c r="K9" s="14"/>
     </row>
-    <row r="10" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>303</v>
       </c>
@@ -3477,7 +3589,7 @@
       </c>
       <c r="K10" s="14"/>
     </row>
-    <row r="11" spans="1:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="15" t="s">
         <v>321</v>
       </c>
@@ -3494,7 +3606,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
     </row>
-    <row r="12" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="61.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="17" t="s">
         <v>323</v>
       </c>
@@ -3513,7 +3625,7 @@
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
     </row>
-    <row r="13" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>304</v>
       </c>
@@ -3530,7 +3642,7 @@
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>305</v>
       </c>
@@ -3560,25 +3672,25 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="26.21875" customWidth="1"/>
-    <col min="2" max="2" width="36.5546875" customWidth="1"/>
-    <col min="3" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="9" width="8.88671875" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.20703125" customWidth="1"/>
+    <col min="2" max="2" width="36.5234375" customWidth="1"/>
+    <col min="3" max="4" width="15.68359375" customWidth="1"/>
+    <col min="5" max="5" width="10.41796875" customWidth="1"/>
+    <col min="6" max="6" width="11.1015625" customWidth="1"/>
+    <col min="7" max="7" width="10.7890625" customWidth="1"/>
+    <col min="8" max="9" width="8.89453125" customWidth="1"/>
+    <col min="10" max="10" width="17.41796875" customWidth="1"/>
+    <col min="11" max="11" width="20.41796875" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="18.77734375" customWidth="1"/>
-    <col min="14" max="14" width="13.44140625" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="18.7890625" customWidth="1"/>
+    <col min="14" max="14" width="13.41796875" customWidth="1"/>
+    <col min="15" max="15" width="11.3125" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
         <v>157</v>
       </c>
@@ -3622,7 +3734,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="51.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -3638,7 +3750,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:16" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="49.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>165</v>
       </c>
@@ -3660,7 +3772,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -3682,7 +3794,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="46.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>168</v>
       </c>
@@ -3710,7 +3822,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>170</v>
       </c>
@@ -3740,7 +3852,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="J7" s="4" t="s">
         <v>175</v>
       </c>
@@ -3759,7 +3871,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
         <v>180</v>
       </c>
@@ -3770,7 +3882,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="41.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4" t="s">
         <v>183</v>
       </c>
@@ -3792,7 +3904,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="5" t="s">
         <v>184</v>
       </c>
@@ -3818,7 +3930,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="5" t="s">
         <v>187</v>
       </c>
@@ -3844,7 +3956,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5" t="s">
         <v>189</v>
       </c>
@@ -3870,7 +3982,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4" t="s">
         <v>191</v>
       </c>
@@ -3894,7 +4006,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
         <v>194</v>
       </c>
@@ -3920,7 +4032,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4" t="s">
         <v>196</v>
       </c>
@@ -3940,7 +4052,7 @@
         <v>900000</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4" t="s">
         <v>198</v>
       </c>
@@ -3962,18 +4074,18 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.68359375" customWidth="1"/>
+    <col min="2" max="2" width="20.7890625" customWidth="1"/>
+    <col min="3" max="3" width="24.5234375" customWidth="1"/>
+    <col min="4" max="4" width="13.89453125" customWidth="1"/>
+    <col min="5" max="5" width="13.41796875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="58.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>199</v>
       </c>
@@ -3996,7 +4108,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="108" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>206</v>
       </c>
@@ -4019,7 +4131,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="103.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>212</v>
       </c>
@@ -4042,7 +4154,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="118.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="118.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>219</v>
       </c>
@@ -4065,7 +4177,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="139.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="139.19999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>225</v>
       </c>
@@ -4088,7 +4200,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="100.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>231</v>
       </c>
@@ -4111,7 +4223,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
         <v>238</v>
       </c>

</xml_diff>